<commit_message>
Mais dados na base de dados
</commit_message>
<xml_diff>
--- a/move-acess/src/main/resources/base.xlsx
+++ b/move-acess/src/main/resources/base.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18f6fa01788ef6bb/Documents/Semestre 2/MoveAcess/web-data-viz/src/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18f6fa01788ef6bb/Documents/Semestre 2/java/move-acess/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_BA723AEB6D74F476CFFF996B8754A19F82B06826" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04B558E6-D87A-4515-86A9-13B576E91516}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_BA723AEB6D74F476CFFF996B8754A19F82B06826" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B90B73D-6BB3-4550-8035-05200FCC6A52}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="213">
   <si>
     <t>Estação</t>
   </si>
@@ -579,18 +579,118 @@
   </si>
   <si>
     <t>Sinalização visual de embarque (Insuficiente)</t>
+  </si>
+  <si>
+    <t>Vila Maria</t>
+  </si>
+  <si>
+    <t>Elevador (inoperante), Rampa, Piso Tátil</t>
+  </si>
+  <si>
+    <t>Elevador (operante), Rampa, Piso Tátil</t>
+  </si>
+  <si>
+    <t>Totalmente Adaptado</t>
+  </si>
+  <si>
+    <t>Santa Cecília</t>
+  </si>
+  <si>
+    <t>Elevador, Rampa, Sanitário Acessível</t>
+  </si>
+  <si>
+    <t>Elevador (inoperante), Rampa</t>
+  </si>
+  <si>
+    <t>Jardim São Paulo</t>
+  </si>
+  <si>
+    <t>Elevador (pendente), Rampa</t>
+  </si>
+  <si>
+    <t>Elevador, Rampa, Piso Tátil</t>
+  </si>
+  <si>
+    <t>Tatuapé (ônibus)</t>
+  </si>
+  <si>
+    <t>297T-10</t>
+  </si>
+  <si>
+    <t>Piso Baixo, Rampa, Espaço Reservado</t>
+  </si>
+  <si>
+    <t>Brás (ônibus)</t>
+  </si>
+  <si>
+    <t>4118-10</t>
+  </si>
+  <si>
+    <t>Pinheiros</t>
+  </si>
+  <si>
+    <t>Elevador (inoperante), Rampa, Telefone para Surdos</t>
+  </si>
+  <si>
+    <t>Elevador, Rampa, Telefone para Surdos</t>
+  </si>
+  <si>
+    <t>Barra Funda</t>
+  </si>
+  <si>
+    <t>Sé</t>
+  </si>
+  <si>
+    <t>Elevador (inoperante), Rampa, Sanitário Acessível</t>
+  </si>
+  <si>
+    <t>República</t>
+  </si>
+  <si>
+    <t>Jabaquara (ônibus)</t>
+  </si>
+  <si>
+    <t>675A-10</t>
+  </si>
+  <si>
+    <t>Morumbi (ônibus)</t>
+  </si>
+  <si>
+    <t>775J-10</t>
+  </si>
+  <si>
+    <t>3 | 7 | 8</t>
+  </si>
+  <si>
+    <t>4 | 7 | 8</t>
+  </si>
+  <si>
+    <t>5 | 7 | 8</t>
+  </si>
+  <si>
+    <t>1 | 3</t>
+  </si>
+  <si>
+    <t>3 | 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -605,6 +705,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,12 +751,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F595"/>
+  <dimension ref="A1:H629"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="F216" sqref="F216"/>
+    <sheetView tabSelected="1" topLeftCell="A503" workbookViewId="0">
+      <selection activeCell="H522" sqref="H522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -9672,7 +9779,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="513" spans="1:5">
+    <row r="513" spans="1:8">
       <c r="A513" t="s">
         <v>159</v>
       </c>
@@ -9689,7 +9796,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="514" spans="1:5">
+    <row r="514" spans="1:8">
       <c r="A514" t="s">
         <v>159</v>
       </c>
@@ -9706,7 +9813,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="515" spans="1:5">
+    <row r="515" spans="1:8">
       <c r="A515" t="s">
         <v>159</v>
       </c>
@@ -9723,7 +9830,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="516" spans="1:5">
+    <row r="516" spans="1:8">
       <c r="A516" t="s">
         <v>159</v>
       </c>
@@ -9740,7 +9847,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="517" spans="1:5">
+    <row r="517" spans="1:8">
       <c r="A517" t="s">
         <v>159</v>
       </c>
@@ -9757,7 +9864,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="518" spans="1:5">
+    <row r="518" spans="1:8">
       <c r="A518" t="s">
         <v>161</v>
       </c>
@@ -9774,7 +9881,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="519" spans="1:5">
+    <row r="519" spans="1:8">
       <c r="A519" t="s">
         <v>161</v>
       </c>
@@ -9791,7 +9898,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="520" spans="1:5">
+    <row r="520" spans="1:8">
       <c r="A520" t="s">
         <v>161</v>
       </c>
@@ -9808,7 +9915,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="521" spans="1:5">
+    <row r="521" spans="1:8">
       <c r="A521" t="s">
         <v>161</v>
       </c>
@@ -9825,7 +9932,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="522" spans="1:5">
+    <row r="522" spans="1:8">
       <c r="A522" t="s">
         <v>161</v>
       </c>
@@ -9841,8 +9948,9 @@
       <c r="E522">
         <v>2023</v>
       </c>
-    </row>
-    <row r="523" spans="1:5">
+      <c r="H522" s="2"/>
+    </row>
+    <row r="523" spans="1:8">
       <c r="A523" t="s">
         <v>161</v>
       </c>
@@ -9859,7 +9967,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="524" spans="1:5">
+    <row r="524" spans="1:8">
       <c r="A524" t="s">
         <v>163</v>
       </c>
@@ -9876,7 +9984,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="525" spans="1:5">
+    <row r="525" spans="1:8">
       <c r="A525" t="s">
         <v>163</v>
       </c>
@@ -9893,7 +10001,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="526" spans="1:5">
+    <row r="526" spans="1:8">
       <c r="A526" t="s">
         <v>163</v>
       </c>
@@ -9910,7 +10018,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="527" spans="1:5">
+    <row r="527" spans="1:8">
       <c r="A527" t="s">
         <v>163</v>
       </c>
@@ -9927,7 +10035,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="528" spans="1:5">
+    <row r="528" spans="1:8">
       <c r="A528" t="s">
         <v>163</v>
       </c>
@@ -11083,7 +11191,586 @@
         <v>2024</v>
       </c>
     </row>
+    <row r="596" spans="1:5">
+      <c r="A596" t="s">
+        <v>182</v>
+      </c>
+      <c r="B596">
+        <v>1</v>
+      </c>
+      <c r="C596" t="s">
+        <v>183</v>
+      </c>
+      <c r="D596" t="s">
+        <v>9</v>
+      </c>
+      <c r="E596">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5">
+      <c r="A597" t="s">
+        <v>182</v>
+      </c>
+      <c r="B597">
+        <v>1</v>
+      </c>
+      <c r="C597" t="s">
+        <v>183</v>
+      </c>
+      <c r="D597" t="s">
+        <v>9</v>
+      </c>
+      <c r="E597">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5">
+      <c r="A598" t="s">
+        <v>182</v>
+      </c>
+      <c r="B598">
+        <v>1</v>
+      </c>
+      <c r="C598" t="s">
+        <v>184</v>
+      </c>
+      <c r="D598" t="s">
+        <v>185</v>
+      </c>
+      <c r="E598">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5">
+      <c r="A599" t="s">
+        <v>186</v>
+      </c>
+      <c r="B599">
+        <v>1</v>
+      </c>
+      <c r="C599" t="s">
+        <v>187</v>
+      </c>
+      <c r="D599" t="s">
+        <v>8</v>
+      </c>
+      <c r="E599">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5">
+      <c r="A600" t="s">
+        <v>186</v>
+      </c>
+      <c r="B600">
+        <v>1</v>
+      </c>
+      <c r="C600" t="s">
+        <v>188</v>
+      </c>
+      <c r="D600" t="s">
+        <v>9</v>
+      </c>
+      <c r="E600">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5">
+      <c r="A601" t="s">
+        <v>186</v>
+      </c>
+      <c r="B601">
+        <v>1</v>
+      </c>
+      <c r="C601" t="s">
+        <v>187</v>
+      </c>
+      <c r="D601" t="s">
+        <v>185</v>
+      </c>
+      <c r="E601">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5">
+      <c r="A602" t="s">
+        <v>189</v>
+      </c>
+      <c r="B602">
+        <v>1</v>
+      </c>
+      <c r="C602" t="s">
+        <v>190</v>
+      </c>
+      <c r="D602" t="s">
+        <v>12</v>
+      </c>
+      <c r="E602">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="603" spans="1:5">
+      <c r="A603" t="s">
+        <v>189</v>
+      </c>
+      <c r="B603">
+        <v>1</v>
+      </c>
+      <c r="C603" t="s">
+        <v>188</v>
+      </c>
+      <c r="D603" t="s">
+        <v>9</v>
+      </c>
+      <c r="E603">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5">
+      <c r="A604" t="s">
+        <v>189</v>
+      </c>
+      <c r="B604">
+        <v>1</v>
+      </c>
+      <c r="C604" t="s">
+        <v>191</v>
+      </c>
+      <c r="D604" t="s">
+        <v>185</v>
+      </c>
+      <c r="E604">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="605" spans="1:5">
+      <c r="A605" t="s">
+        <v>192</v>
+      </c>
+      <c r="B605" t="s">
+        <v>193</v>
+      </c>
+      <c r="C605" t="s">
+        <v>194</v>
+      </c>
+      <c r="D605" t="s">
+        <v>8</v>
+      </c>
+      <c r="E605">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5">
+      <c r="A606" t="s">
+        <v>192</v>
+      </c>
+      <c r="B606" t="s">
+        <v>193</v>
+      </c>
+      <c r="C606" t="s">
+        <v>194</v>
+      </c>
+      <c r="D606" t="s">
+        <v>8</v>
+      </c>
+      <c r="E606">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5">
+      <c r="A607" t="s">
+        <v>192</v>
+      </c>
+      <c r="B607" t="s">
+        <v>193</v>
+      </c>
+      <c r="C607" t="s">
+        <v>194</v>
+      </c>
+      <c r="D607" t="s">
+        <v>8</v>
+      </c>
+      <c r="E607">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5">
+      <c r="A608" t="s">
+        <v>195</v>
+      </c>
+      <c r="B608" t="s">
+        <v>196</v>
+      </c>
+      <c r="C608" t="s">
+        <v>194</v>
+      </c>
+      <c r="D608" t="s">
+        <v>8</v>
+      </c>
+      <c r="E608">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="609" spans="1:5">
+      <c r="A609" t="s">
+        <v>195</v>
+      </c>
+      <c r="B609" t="s">
+        <v>196</v>
+      </c>
+      <c r="C609" t="s">
+        <v>194</v>
+      </c>
+      <c r="D609" t="s">
+        <v>8</v>
+      </c>
+      <c r="E609">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="610" spans="1:5">
+      <c r="A610" t="s">
+        <v>195</v>
+      </c>
+      <c r="B610" t="s">
+        <v>196</v>
+      </c>
+      <c r="C610" t="s">
+        <v>194</v>
+      </c>
+      <c r="D610" t="s">
+        <v>8</v>
+      </c>
+      <c r="E610">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="611" spans="1:5">
+      <c r="A611" t="s">
+        <v>197</v>
+      </c>
+      <c r="B611">
+        <v>4</v>
+      </c>
+      <c r="C611" t="s">
+        <v>198</v>
+      </c>
+      <c r="D611" t="s">
+        <v>9</v>
+      </c>
+      <c r="E611">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="612" spans="1:5">
+      <c r="A612" t="s">
+        <v>197</v>
+      </c>
+      <c r="B612">
+        <v>4</v>
+      </c>
+      <c r="C612" t="s">
+        <v>198</v>
+      </c>
+      <c r="D612" t="s">
+        <v>9</v>
+      </c>
+      <c r="E612">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="613" spans="1:5">
+      <c r="A613" t="s">
+        <v>197</v>
+      </c>
+      <c r="B613">
+        <v>4</v>
+      </c>
+      <c r="C613" t="s">
+        <v>199</v>
+      </c>
+      <c r="D613" t="s">
+        <v>185</v>
+      </c>
+      <c r="E613">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="614" spans="1:5">
+      <c r="A614" t="s">
+        <v>197</v>
+      </c>
+      <c r="B614">
+        <v>4</v>
+      </c>
+      <c r="C614" t="s">
+        <v>199</v>
+      </c>
+      <c r="D614" t="s">
+        <v>8</v>
+      </c>
+      <c r="E614">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="615" spans="1:5">
+      <c r="A615" t="s">
+        <v>200</v>
+      </c>
+      <c r="B615" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C615" t="s">
+        <v>183</v>
+      </c>
+      <c r="D615" t="s">
+        <v>9</v>
+      </c>
+      <c r="E615">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="616" spans="1:5">
+      <c r="A616" t="s">
+        <v>200</v>
+      </c>
+      <c r="B616" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C616" t="s">
+        <v>183</v>
+      </c>
+      <c r="D616" t="s">
+        <v>9</v>
+      </c>
+      <c r="E616">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="617" spans="1:5">
+      <c r="A617" t="s">
+        <v>200</v>
+      </c>
+      <c r="B617" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C617" t="s">
+        <v>191</v>
+      </c>
+      <c r="D617" t="s">
+        <v>185</v>
+      </c>
+      <c r="E617">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="618" spans="1:5">
+      <c r="A618" t="s">
+        <v>201</v>
+      </c>
+      <c r="B618" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C618" t="s">
+        <v>202</v>
+      </c>
+      <c r="D618" t="s">
+        <v>9</v>
+      </c>
+      <c r="E618">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5">
+      <c r="A619" t="s">
+        <v>201</v>
+      </c>
+      <c r="B619" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C619" t="s">
+        <v>202</v>
+      </c>
+      <c r="D619" t="s">
+        <v>9</v>
+      </c>
+      <c r="E619">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="620" spans="1:5">
+      <c r="A620" t="s">
+        <v>201</v>
+      </c>
+      <c r="B620" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C620" t="s">
+        <v>187</v>
+      </c>
+      <c r="D620" t="s">
+        <v>185</v>
+      </c>
+      <c r="E620">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5">
+      <c r="A621" t="s">
+        <v>203</v>
+      </c>
+      <c r="B621" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C621" t="s">
+        <v>188</v>
+      </c>
+      <c r="D621" t="s">
+        <v>9</v>
+      </c>
+      <c r="E621">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5">
+      <c r="A622" t="s">
+        <v>203</v>
+      </c>
+      <c r="B622" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C622" t="s">
+        <v>191</v>
+      </c>
+      <c r="D622" t="s">
+        <v>185</v>
+      </c>
+      <c r="E622">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5">
+      <c r="A623" t="s">
+        <v>203</v>
+      </c>
+      <c r="B623" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C623" t="s">
+        <v>191</v>
+      </c>
+      <c r="D623" t="s">
+        <v>8</v>
+      </c>
+      <c r="E623">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5">
+      <c r="A624" t="s">
+        <v>204</v>
+      </c>
+      <c r="B624" t="s">
+        <v>205</v>
+      </c>
+      <c r="C624" t="s">
+        <v>194</v>
+      </c>
+      <c r="D624" t="s">
+        <v>8</v>
+      </c>
+      <c r="E624">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5">
+      <c r="A625" t="s">
+        <v>204</v>
+      </c>
+      <c r="B625" t="s">
+        <v>205</v>
+      </c>
+      <c r="C625" t="s">
+        <v>194</v>
+      </c>
+      <c r="D625" t="s">
+        <v>8</v>
+      </c>
+      <c r="E625">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5">
+      <c r="A626" t="s">
+        <v>204</v>
+      </c>
+      <c r="B626" t="s">
+        <v>205</v>
+      </c>
+      <c r="C626" t="s">
+        <v>194</v>
+      </c>
+      <c r="D626" t="s">
+        <v>8</v>
+      </c>
+      <c r="E626">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5">
+      <c r="A627" t="s">
+        <v>206</v>
+      </c>
+      <c r="B627" t="s">
+        <v>207</v>
+      </c>
+      <c r="C627" t="s">
+        <v>194</v>
+      </c>
+      <c r="D627" t="s">
+        <v>8</v>
+      </c>
+      <c r="E627">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5">
+      <c r="A628" t="s">
+        <v>206</v>
+      </c>
+      <c r="B628" t="s">
+        <v>207</v>
+      </c>
+      <c r="C628" t="s">
+        <v>194</v>
+      </c>
+      <c r="D628" t="s">
+        <v>8</v>
+      </c>
+      <c r="E628">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5">
+      <c r="A629" t="s">
+        <v>206</v>
+      </c>
+      <c r="B629" t="s">
+        <v>207</v>
+      </c>
+      <c r="C629" t="s">
+        <v>194</v>
+      </c>
+      <c r="D629" t="s">
+        <v>8</v>
+      </c>
+      <c r="E629">
+        <v>2022</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>